<commit_message>
Inclusão do evento de concluir OS
</commit_message>
<xml_diff>
--- a/TCC - Monografia/Documentos/Últimas versões EAP/Modelo de Análise dos Eventos.xlsx
+++ b/TCC - Monografia/Documentos/Últimas versões EAP/Modelo de Análise dos Eventos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4170"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4170" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Capacidades</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>O Gerente Operacional encaminha as informações para o Administrativo  no final da semana</t>
   </si>
   <si>
     <t xml:space="preserve">A atendente recebe o pedido e armazena as informações 
@@ -124,6 +121,27 @@
   </si>
   <si>
     <t>Gerente Operacional efetua a impressão da OS para a realização do serviço.</t>
+  </si>
+  <si>
+    <t>O Gerente de Manutenção encaminha as informações para o Administrativo  no final da semana</t>
+  </si>
+  <si>
+    <t>Concluir OS</t>
+  </si>
+  <si>
+    <t>Motoboy entrega ao gerente operacional as O.S. realizadas para validação</t>
+  </si>
+  <si>
+    <t>Gerente Operacional registra os pontos do motoboy para posterior pagamento</t>
+  </si>
+  <si>
+    <t>Gerente Operacional registra os pontos para cobrança do cliente</t>
+  </si>
+  <si>
+    <t>X(FB7)</t>
+  </si>
+  <si>
+    <t>X(FB8)</t>
   </si>
 </sst>
 </file>
@@ -305,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -398,6 +416,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -771,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
@@ -854,7 +890,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -872,7 +908,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -894,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
@@ -912,7 +948,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -930,7 +966,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -972,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="A1:J8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,7 +1097,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1074,7 +1110,7 @@
     </row>
     <row r="5" spans="1:10" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>15</v>
@@ -1083,7 +1119,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
@@ -1096,7 +1132,7 @@
     </row>
     <row r="6" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>15</v>
@@ -1105,7 +1141,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
@@ -1118,7 +1154,7 @@
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>15</v>
@@ -1127,7 +1163,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
@@ -1140,7 +1176,7 @@
     </row>
     <row r="8" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -1149,21 +1185,81 @@
         <v>6</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="12"/>
     </row>
+    <row r="9" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="13">
+        <v>7</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="13">
+        <v>8</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="13">
+        <v>9</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Alterei o meu evento, deixei entre colchetes para ver se todos concordam
</commit_message>
<xml_diff>
--- a/TCC - Monografia/Documentos/Últimas versões EAP/Modelo de Análise dos Eventos.xlsx
+++ b/TCC - Monografia/Documentos/Últimas versões EAP/Modelo de Análise dos Eventos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Desktop\pos-fit-es10\trunk\TCC - Monografia\Documentos\Últimas versões EAP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4170" activeTab="2"/>
   </bookViews>
@@ -66,9 +71,6 @@
     <t>FB</t>
   </si>
   <si>
-    <t>Motoboy passa as informações sobre a manutenção realizada em um determinado dia</t>
-  </si>
-  <si>
     <t>Consultar Manutenção</t>
   </si>
   <si>
@@ -123,9 +125,6 @@
     <t>Gerente Operacional efetua a impressão da OS para a realização do serviço.</t>
   </si>
   <si>
-    <t>O Gerente de Manutenção encaminha as informações para o Administrativo  no final da semana</t>
-  </si>
-  <si>
     <t>Concluir OS</t>
   </si>
   <si>
@@ -142,6 +141,12 @@
   </si>
   <si>
     <t>X(FB8)</t>
+  </si>
+  <si>
+    <t>Motoboy passa as informações sobre a manutenção realizada no veículo</t>
+  </si>
+  <si>
+    <t>O Gerente de Manutenção [disponibiliza as manutenções realizadas para o Administrativo] encaminha as informações para o Administrativo  no final da semana</t>
   </si>
 </sst>
 </file>
@@ -561,7 +566,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,7 +601,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -872,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
@@ -890,7 +895,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -908,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -930,7 +935,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
@@ -948,7 +953,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -966,7 +971,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -1010,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,11 +1080,11 @@
         <v>1</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -1088,7 +1093,7 @@
     </row>
     <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>15</v>
@@ -1097,20 +1102,20 @@
         <v>2</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>15</v>
@@ -1119,11 +1124,11 @@
         <v>3</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -1132,7 +1137,7 @@
     </row>
     <row r="6" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>15</v>
@@ -1141,11 +1146,11 @@
         <v>4</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -1154,7 +1159,7 @@
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>15</v>
@@ -1163,11 +1168,11 @@
         <v>5</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1176,7 +1181,7 @@
     </row>
     <row r="8" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>15</v>
@@ -1185,12 +1190,12 @@
         <v>6</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -1198,7 +1203,7 @@
     </row>
     <row r="9" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="35" t="s">
         <v>15</v>
@@ -1207,11 +1212,11 @@
         <v>7</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1225,12 +1230,12 @@
         <v>8</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -1243,12 +1248,12 @@
         <v>9</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>

</xml_diff>